<commit_message>
updateForm- css수정 header- admin 전용로고 생성
</commit_message>
<xml_diff>
--- a/20220531_FunctionalDescription 진수빈.xlsx
+++ b/20220531_FunctionalDescription 진수빈.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anfzh\Desktop\IDEA\spring_framework\CheersMall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180B8946-159C-4F80-8929-A9482C27ED57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B116C0-8298-427E-B35A-05EC52FCA57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="969" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2201,45 +2201,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2254,6 +2215,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2617,8 +2617,8 @@
   </sheetPr>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2642,40 +2642,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="39.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="E2" s="30" t="s">
+      <c r="B2" s="24"/>
+      <c r="E2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="30"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
@@ -2683,61 +2683,61 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21" t="s">
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="7" t="s">
         <v>18</v>
       </c>
@@ -2750,13 +2750,13 @@
       <c r="O5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="21"/>
+      <c r="P5" s="25"/>
     </row>
     <row r="6" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="30" t="s">
         <v>179</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2791,8 +2791,8 @@
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
@@ -2831,8 +2831,8 @@
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2873,8 +2873,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="3" t="s">
         <v>48</v>
       </c>
@@ -2913,8 +2913,8 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="3" t="s">
         <v>54</v>
       </c>
@@ -2957,8 +2957,8 @@
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="3" t="s">
         <v>56</v>
       </c>
@@ -2997,8 +2997,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="3" t="s">
         <v>60</v>
       </c>
@@ -3041,8 +3041,8 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="3" t="s">
         <v>67</v>
       </c>
@@ -3081,8 +3081,8 @@
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3115,8 +3115,8 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="3" t="s">
         <v>74</v>
       </c>
@@ -3159,8 +3159,8 @@
       <c r="P15" s="3"/>
     </row>
     <row r="16" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="3" t="s">
         <v>79</v>
       </c>
@@ -3197,12 +3197,12 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="20" t="s">
         <v>117</v>
       </c>
       <c r="E17" s="3"/>
@@ -3227,12 +3227,12 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="20" t="s">
         <v>118</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -3263,10 +3263,10 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="33" t="s">
         <v>84</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -3297,8 +3297,8 @@
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="19"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="3" t="s">
         <v>171</v>
       </c>
@@ -3331,8 +3331,8 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="19"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="3" t="s">
         <v>172</v>
       </c>
@@ -3371,8 +3371,8 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="19"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="3" t="s">
         <v>173</v>
       </c>
@@ -3382,7 +3382,7 @@
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="18" t="s">
         <v>150</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -3415,12 +3415,12 @@
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="19"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="20" t="s">
         <v>181</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -3459,12 +3459,12 @@
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="19"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="20" t="s">
         <v>184</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -3499,12 +3499,12 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="19"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="20" t="s">
         <v>185</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -3539,12 +3539,12 @@
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="20"/>
-      <c r="B26" s="24"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="20" t="s">
         <v>186</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -3579,16 +3579,16 @@
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="33" t="s">
         <v>179</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="19" t="s">
         <v>203</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -3627,12 +3627,12 @@
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="19"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="21" t="s">
         <v>99</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -3671,12 +3671,12 @@
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="19"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="34"/>
       <c r="C29" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="22" t="s">
         <v>93</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -3715,8 +3715,8 @@
       <c r="P29" s="3"/>
     </row>
     <row r="30" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="19"/>
-      <c r="B30" s="22" t="s">
+      <c r="A30" s="31"/>
+      <c r="B30" s="33" t="s">
         <v>84</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -3751,8 +3751,8 @@
       <c r="P30" s="3"/>
     </row>
     <row r="31" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="19"/>
-      <c r="B31" s="23"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="3" t="s">
         <v>165</v>
       </c>
@@ -3795,12 +3795,12 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="19"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="14" t="s">
         <v>140</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -3839,8 +3839,8 @@
       <c r="P32" s="3"/>
     </row>
     <row r="33" spans="1:16" s="13" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="19"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="3" t="s">
         <v>167</v>
       </c>
@@ -3873,8 +3873,8 @@
       <c r="P33" s="3"/>
     </row>
     <row r="34" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="19"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="3" t="s">
         <v>168</v>
       </c>
@@ -3917,8 +3917,8 @@
       <c r="P34" s="3"/>
     </row>
     <row r="35" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="20"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="3" t="s">
         <v>169</v>
       </c>
@@ -3955,10 +3955,10 @@
       <c r="P35" s="3"/>
     </row>
     <row r="36" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="30" t="s">
         <v>180</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -4005,8 +4005,8 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="3" t="s">
         <v>154</v>
       </c>
@@ -4051,8 +4051,8 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="3" t="s">
         <v>155</v>
       </c>
@@ -4095,8 +4095,8 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
       <c r="C39" s="3" t="s">
         <v>156</v>
       </c>
@@ -4470,6 +4470,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="A6:A18"/>
+    <mergeCell ref="B6:B18"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A27:A35"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="L4:O4"/>
@@ -4486,16 +4496,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="A6:A18"/>
-    <mergeCell ref="B6:B18"/>
-    <mergeCell ref="B19:B26"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A27:A35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
댓글 수정- 수정버튼을 입력하면 innerHTML=form,input,button을 넣어준다 입력시   divId.innerHTML='<form action="/comment/update" method="post">'                         +'<input type="text" value="' + itemId + '" name="itemId" readonly>'                         +'<input type="text" value="' + commentId + '" name="commentId" readonly>'                         +'<input type="text" value="'+ commentContents +'" name="commentContents">'                         +'<button>댓글수정</button></form>';                         싱글쿼터를 주의하자
</commit_message>
<xml_diff>
--- a/20220531_FunctionalDescription 진수빈.xlsx
+++ b/20220531_FunctionalDescription 진수빈.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anfzh\Desktop\IDEA\spring_framework\CheersMall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502C60B1-42AE-49E4-AC8B-2E649D1F360E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578C4117-9B8D-4EE8-866F-097A1FA4E80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="25760" windowHeight="15440" tabRatio="969" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="969" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Functional_Description" sheetId="36" r:id="rId1"/>
@@ -2216,6 +2216,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2225,9 +2249,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2236,27 +2257,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2620,8 +2620,8 @@
   </sheetPr>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2645,40 +2645,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="39.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" ht="17.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="E2" s="35" t="s">
+      <c r="B2" s="25"/>
+      <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
@@ -2692,7 +2692,7 @@
       <c r="B4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -2704,13 +2704,13 @@
       <c r="F4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="28" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="27" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="26" t="s">
@@ -2732,11 +2732,11 @@
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
-      <c r="C5" s="32"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
       <c r="F5" s="26"/>
-      <c r="G5" s="34"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
@@ -2756,10 +2756,10 @@
       <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="31" t="s">
         <v>179</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2794,8 +2794,8 @@
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
@@ -2834,8 +2834,8 @@
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
@@ -2876,8 +2876,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="3" t="s">
         <v>48</v>
       </c>
@@ -2916,8 +2916,8 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="3" t="s">
         <v>54</v>
       </c>
@@ -2960,8 +2960,8 @@
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="3" t="s">
         <v>56</v>
       </c>
@@ -3000,8 +3000,8 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="3" t="s">
         <v>60</v>
       </c>
@@ -3044,8 +3044,8 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="3" t="s">
         <v>67</v>
       </c>
@@ -3084,8 +3084,8 @@
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3118,8 +3118,8 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="3" t="s">
         <v>74</v>
       </c>
@@ -3162,8 +3162,8 @@
       <c r="P15" s="3"/>
     </row>
     <row r="16" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="3" t="s">
         <v>79</v>
       </c>
@@ -3200,12 +3200,12 @@
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E17" s="3"/>
@@ -3230,8 +3230,8 @@
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="3" t="s">
         <v>114</v>
       </c>
@@ -3266,10 +3266,10 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="34" t="s">
         <v>84</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -3300,8 +3300,8 @@
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="24"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="3" t="s">
         <v>171</v>
       </c>
@@ -3334,8 +3334,8 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="24"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="3" t="s">
         <v>172</v>
       </c>
@@ -3374,8 +3374,8 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="24"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="3" t="s">
         <v>173</v>
       </c>
@@ -3418,8 +3418,8 @@
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="24"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="3" t="s">
         <v>174</v>
       </c>
@@ -3462,8 +3462,8 @@
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="24"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="3" t="s">
         <v>175</v>
       </c>
@@ -3502,8 +3502,8 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="24"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="3" t="s">
         <v>176</v>
       </c>
@@ -3542,8 +3542,8 @@
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="25"/>
-      <c r="B26" s="29"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="3" t="s">
         <v>177</v>
       </c>
@@ -3582,10 +3582,10 @@
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="34" t="s">
         <v>179</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -3630,8 +3630,8 @@
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="24"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="3" t="s">
         <v>162</v>
       </c>
@@ -3674,8 +3674,8 @@
       <c r="P28" s="3"/>
     </row>
     <row r="29" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="24"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="3" t="s">
         <v>163</v>
       </c>
@@ -3718,8 +3718,8 @@
       <c r="P29" s="3"/>
     </row>
     <row r="30" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="24"/>
-      <c r="B30" s="27" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="34" t="s">
         <v>84</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -3754,8 +3754,8 @@
       <c r="P30" s="3"/>
     </row>
     <row r="31" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="24"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="3" t="s">
         <v>165</v>
       </c>
@@ -3798,8 +3798,8 @@
       <c r="P31" s="3"/>
     </row>
     <row r="32" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="24"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="3" t="s">
         <v>166</v>
       </c>
@@ -3842,8 +3842,8 @@
       <c r="P32" s="3"/>
     </row>
     <row r="33" spans="1:16" s="13" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="24"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="3" t="s">
         <v>167</v>
       </c>
@@ -3876,8 +3876,8 @@
       <c r="P33" s="3"/>
     </row>
     <row r="34" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="24"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="3" t="s">
         <v>168</v>
       </c>
@@ -3920,8 +3920,8 @@
       <c r="P34" s="3"/>
     </row>
     <row r="35" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="25"/>
-      <c r="B35" s="29"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="3" t="s">
         <v>169</v>
       </c>
@@ -3958,16 +3958,16 @@
       <c r="P35" s="3"/>
     </row>
     <row r="36" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="31" t="s">
         <v>180</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="14" t="s">
         <v>111</v>
       </c>
       <c r="E36" s="3" t="s">
@@ -4008,12 +4008,12 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="14" t="s">
         <v>113</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -4054,12 +4054,12 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="15" t="s">
         <v>211</v>
       </c>
       <c r="E38" s="3"/>
@@ -4098,12 +4098,12 @@
       </c>
     </row>
     <row r="39" spans="1:16" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="14" t="s">
         <v>112</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -4473,6 +4473,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="A6:A18"/>
+    <mergeCell ref="B6:B18"/>
+    <mergeCell ref="B19:B26"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B35"/>
+    <mergeCell ref="A27:A35"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="L4:O4"/>
@@ -4489,16 +4499,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="A6:A18"/>
-    <mergeCell ref="B6:B18"/>
-    <mergeCell ref="B19:B26"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B35"/>
-    <mergeCell ref="A27:A35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>